<commit_message>
Updated code and updated metadata
</commit_message>
<xml_diff>
--- a/dataset_metadata.xlsx
+++ b/dataset_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uibes-my.sharepoint.com/personal/agc968_id_uib_eu/Documents/TFG/PycharmProjects/GEEIA-TFG-DFU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{D3773089-7DAF-44F1-9F4B-4D9CCE4173E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C71CF293-DF41-4700-89E3-4058FDF6D75A}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{D3773089-7DAF-44F1-9F4B-4D9CCE4173E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0641FE81-EB1F-4C18-A5E0-192FC413F733}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" tabRatio="601" xr2:uid="{14AC8030-20A7-4C66-8027-B1BAD1A4B756}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="26010" windowHeight="10545" tabRatio="601" xr2:uid="{14AC8030-20A7-4C66-8027-B1BAD1A4B756}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -323,9 +323,6 @@
     <t>[{"start_frame":832,"end_frame":841}]</t>
   </si>
   <si>
-    <t>[{"type":"STAFF","appearances":[{"start":{"frame":116,"landmarks":{"right_eye":[256,485],"nose":[234,483],"mouth_right":[240,457],"mouth_left":[215,470]}},"end":{"frame":227}}]},{"type":"PATIENT","appearances":[{"start":{"frame":796,"landmarks":{"left_eye":[666,-3],"nose":[636,2],"mouth_right":[626,14],"mouth_left":[645,25]}},"end":{"frame":841}}]}]</t>
-  </si>
-  <si>
     <t>patient_id</t>
   </si>
   <si>
@@ -354,6 +351,9 @@
   </si>
   <si>
     <t>person_appearances</t>
+  </si>
+  <si>
+    <t>[{"type":"STAFF","appearances":[{"start":{"frame":116,"landmarks":{"right_eye":[256,485],"nose":[234,483],"mouth_right":[240,457],"mouth_left":[215,470]}},"end":{"frame":228}},{"start":{"frame":260,"landmarks":{"mouth_right":[252,471]}},"end":{"frame":279}}]},{"type":"PATIENT","appearances":[{"start":{"frame":796,"landmarks":{"left_eye":[666,-3],"nose":[636,2],"mouth_right":[626,14],"mouth_left":[645,25]}},"end":{"frame":841}}]}]</t>
   </si>
 </sst>
 </file>
@@ -602,13 +602,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -964,10 +964,10 @@
   <dimension ref="A1:J75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B65" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomRight" activeCell="L76" sqref="L76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -984,34 +984,34 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B1" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="C1" s="23" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C1" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" s="23" t="s">
+      <c r="F1" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="G1" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="24" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="24" t="s">
         <v>104</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>99</v>
-      </c>
-      <c r="G1" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="H1" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="I1" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="J1" s="24" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1035,7 +1035,7 @@
       <c r="J2" s="12"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="26">
+      <c r="A3" s="27">
         <v>2</v>
       </c>
       <c r="B3" s="16" t="s">
@@ -1055,7 +1055,7 @@
       <c r="J3" s="12"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="26"/>
+      <c r="A4" s="27"/>
       <c r="B4" s="16" t="s">
         <v>2</v>
       </c>
@@ -1075,7 +1075,7 @@
       <c r="J4" s="12"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="26"/>
+      <c r="A5" s="27"/>
       <c r="B5" s="16" t="s">
         <v>3</v>
       </c>
@@ -1207,7 +1207,7 @@
       <c r="J10" s="12"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="27">
+      <c r="A11" s="25">
         <v>8</v>
       </c>
       <c r="B11" s="16" t="s">
@@ -1229,7 +1229,7 @@
       <c r="J11" s="12"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
+      <c r="A12" s="25"/>
       <c r="B12" s="16" t="s">
         <v>10</v>
       </c>
@@ -1249,7 +1249,7 @@
       <c r="J12" s="12"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="27"/>
+      <c r="A13" s="25"/>
       <c r="B13" s="16" t="s">
         <v>11</v>
       </c>
@@ -1359,7 +1359,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="27">
+      <c r="A18" s="25">
         <v>13</v>
       </c>
       <c r="B18" s="16" t="s">
@@ -1379,7 +1379,7 @@
       <c r="J18" s="12"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="27"/>
+      <c r="A19" s="25"/>
       <c r="B19" s="16" t="s">
         <v>17</v>
       </c>
@@ -1399,7 +1399,7 @@
       <c r="J19" s="12"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="27"/>
+      <c r="A20" s="25"/>
       <c r="B20" s="16" t="s">
         <v>18</v>
       </c>
@@ -1413,7 +1413,7 @@
       <c r="J20" s="12"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="25">
+      <c r="A21" s="26">
         <v>14</v>
       </c>
       <c r="B21" s="16" t="s">
@@ -1429,7 +1429,7 @@
       <c r="J21" s="12"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="25"/>
+      <c r="A22" s="26"/>
       <c r="B22" s="16" t="s">
         <v>20</v>
       </c>
@@ -1445,7 +1445,7 @@
       <c r="J22" s="12"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="25"/>
+      <c r="A23" s="26"/>
       <c r="B23" s="16" t="s">
         <v>21</v>
       </c>
@@ -1463,7 +1463,7 @@
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="27">
+      <c r="A24" s="25">
         <v>15</v>
       </c>
       <c r="B24" s="16" t="s">
@@ -1481,7 +1481,7 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="27"/>
+      <c r="A25" s="25"/>
       <c r="B25" s="16" t="s">
         <v>23</v>
       </c>
@@ -1499,7 +1499,7 @@
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="25">
+      <c r="A26" s="26">
         <v>16</v>
       </c>
       <c r="B26" s="16" t="s">
@@ -1515,7 +1515,7 @@
       <c r="J26" s="12"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="25"/>
+      <c r="A27" s="26"/>
       <c r="B27" s="16" t="s">
         <v>25</v>
       </c>
@@ -1531,7 +1531,7 @@
       <c r="J27" s="12"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="25">
+      <c r="A28" s="26">
         <v>17</v>
       </c>
       <c r="B28" s="16" t="s">
@@ -1549,7 +1549,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="25"/>
+      <c r="A29" s="26"/>
       <c r="B29" s="16" t="s">
         <v>27</v>
       </c>
@@ -1565,7 +1565,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="25"/>
+      <c r="A30" s="26"/>
       <c r="B30" s="16" t="s">
         <v>28</v>
       </c>
@@ -1597,7 +1597,7 @@
       <c r="J31" s="12"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="25">
+      <c r="A32" s="26">
         <v>19</v>
       </c>
       <c r="B32" s="16" t="s">
@@ -1617,7 +1617,7 @@
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="25"/>
+      <c r="A33" s="26"/>
       <c r="B33" s="16" t="s">
         <v>31</v>
       </c>
@@ -1633,7 +1633,7 @@
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="25"/>
+      <c r="A34" s="26"/>
       <c r="B34" s="16" t="s">
         <v>32</v>
       </c>
@@ -1651,7 +1651,7 @@
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="27">
+      <c r="A35" s="25">
         <v>20</v>
       </c>
       <c r="B35" s="16" t="s">
@@ -1667,7 +1667,7 @@
       <c r="J35" s="12"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="27"/>
+      <c r="A36" s="25"/>
       <c r="B36" s="16" t="s">
         <v>34</v>
       </c>
@@ -1681,7 +1681,7 @@
       <c r="J36" s="12"/>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="27"/>
+      <c r="A37" s="25"/>
       <c r="B37" s="16" t="s">
         <v>35</v>
       </c>
@@ -1695,7 +1695,7 @@
       <c r="J37" s="12"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="27">
+      <c r="A38" s="25">
         <v>21</v>
       </c>
       <c r="B38" s="16" t="s">
@@ -1713,7 +1713,7 @@
       <c r="J38" s="12"/>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="27"/>
+      <c r="A39" s="25"/>
       <c r="B39" s="16" t="s">
         <v>37</v>
       </c>
@@ -1727,7 +1727,7 @@
       <c r="J39" s="12"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="27"/>
+      <c r="A40" s="25"/>
       <c r="B40" s="16" t="s">
         <v>38</v>
       </c>
@@ -1759,7 +1759,7 @@
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="27">
+      <c r="A42" s="25">
         <v>23</v>
       </c>
       <c r="B42" s="16" t="s">
@@ -1777,7 +1777,7 @@
       <c r="J42" s="12"/>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="27"/>
+      <c r="A43" s="25"/>
       <c r="B43" s="16" t="s">
         <v>41</v>
       </c>
@@ -1793,7 +1793,7 @@
       <c r="J43" s="12"/>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="27"/>
+      <c r="A44" s="25"/>
       <c r="B44" s="16" t="s">
         <v>42</v>
       </c>
@@ -1825,7 +1825,7 @@
       <c r="J45" s="12"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="27">
+      <c r="A46" s="25">
         <v>25</v>
       </c>
       <c r="B46" s="16" t="s">
@@ -1841,7 +1841,7 @@
       <c r="J46" s="12"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="27"/>
+      <c r="A47" s="25"/>
       <c r="B47" s="16" t="s">
         <v>45</v>
       </c>
@@ -1855,7 +1855,7 @@
       <c r="J47" s="12"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="27"/>
+      <c r="A48" s="25"/>
       <c r="B48" s="16" t="s">
         <v>46</v>
       </c>
@@ -1887,7 +1887,7 @@
       <c r="J49" s="12"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" s="27">
+      <c r="A50" s="25">
         <v>27</v>
       </c>
       <c r="B50" s="16" t="s">
@@ -1903,7 +1903,7 @@
       <c r="J50" s="12"/>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" s="27"/>
+      <c r="A51" s="25"/>
       <c r="B51" s="16" t="s">
         <v>49</v>
       </c>
@@ -1917,7 +1917,7 @@
       <c r="J51" s="12"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" s="27"/>
+      <c r="A52" s="25"/>
       <c r="B52" s="16" t="s">
         <v>50</v>
       </c>
@@ -1933,7 +1933,7 @@
       <c r="J52" s="12"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A53" s="27">
+      <c r="A53" s="25">
         <v>28</v>
       </c>
       <c r="B53" s="16" t="s">
@@ -1951,7 +1951,7 @@
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A54" s="27"/>
+      <c r="A54" s="25"/>
       <c r="B54" s="16" t="s">
         <v>52</v>
       </c>
@@ -1967,7 +1967,7 @@
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A55" s="27"/>
+      <c r="A55" s="25"/>
       <c r="B55" s="16" t="s">
         <v>53</v>
       </c>
@@ -2039,7 +2039,7 @@
       <c r="J58" s="12"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A59" s="27">
+      <c r="A59" s="25">
         <v>32</v>
       </c>
       <c r="B59" s="16" t="s">
@@ -2059,7 +2059,7 @@
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A60" s="27"/>
+      <c r="A60" s="25"/>
       <c r="B60" s="16" t="s">
         <v>58</v>
       </c>
@@ -2095,7 +2095,7 @@
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A62" s="27">
+      <c r="A62" s="25">
         <v>34</v>
       </c>
       <c r="B62" s="16" t="s">
@@ -2115,7 +2115,7 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A63" s="27"/>
+      <c r="A63" s="25"/>
       <c r="B63" s="16" t="s">
         <v>61</v>
       </c>
@@ -2169,7 +2169,7 @@
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A66" s="27">
+      <c r="A66" s="25">
         <v>37</v>
       </c>
       <c r="B66" s="16" t="s">
@@ -2189,7 +2189,7 @@
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A67" s="27"/>
+      <c r="A67" s="25"/>
       <c r="B67" s="16" t="s">
         <v>65</v>
       </c>
@@ -2207,7 +2207,7 @@
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A68" s="27"/>
+      <c r="A68" s="25"/>
       <c r="B68" s="16" t="s">
         <v>66</v>
       </c>
@@ -2225,7 +2225,7 @@
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A69" s="27"/>
+      <c r="A69" s="25"/>
       <c r="B69" s="16" t="s">
         <v>67</v>
       </c>
@@ -2241,7 +2241,7 @@
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A70" s="27">
+      <c r="A70" s="25">
         <v>38</v>
       </c>
       <c r="B70" s="16" t="s">
@@ -2259,7 +2259,7 @@
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A71" s="27"/>
+      <c r="A71" s="25"/>
       <c r="B71" s="16" t="s">
         <v>69</v>
       </c>
@@ -2305,7 +2305,7 @@
       <c r="J73" s="12"/>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A74" s="27">
+      <c r="A74" s="25">
         <v>41</v>
       </c>
       <c r="B74" s="16" t="s">
@@ -2351,17 +2351,11 @@
         <v>94</v>
       </c>
       <c r="J75" s="15" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A66:A69"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A11:A13"/>
     <mergeCell ref="A74:A75"/>
     <mergeCell ref="A70:A71"/>
     <mergeCell ref="A18:A20"/>
@@ -2375,6 +2369,12 @@
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="A53:A55"/>
     <mergeCell ref="A28:A30"/>
+    <mergeCell ref="A66:A69"/>
+    <mergeCell ref="A62:A63"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A11:A13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2636,20 +2636,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="b6e30ae0-770c-4ded-9a45-db310f4376cf" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="b6e30ae0-770c-4ded-9a45-db310f4376cf" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2672,14 +2672,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBFD5DB7-20B3-4413-B343-207357287550}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{54E07BE4-568A-4A33-A47A-9A6DE9B672F8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -2694,4 +2686,12 @@
     <ds:schemaRef ds:uri="b6e30ae0-770c-4ded-9a45-db310f4376cf"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EBFD5DB7-20B3-4413-B343-207357287550}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add more prints to show the current status
</commit_message>
<xml_diff>
--- a/dataset_metadata.xlsx
+++ b/dataset_metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uibes-my.sharepoint.com/personal/agc968_id_uib_eu/Documents/TFG/PycharmProjects/GEEIA-TFG-DFU/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uibes-my.sharepoint.com/personal/agc968_id_uib_eu/Documents/TFG/GEEIA-TFG-DFU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="8_{D3773089-7DAF-44F1-9F4B-4D9CCE4173E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{46FBA2DB-672F-42EF-BA41-14F6D57B394C}"/>
+  <xr:revisionPtr revIDLastSave="209" documentId="8_{D3773089-7DAF-44F1-9F4B-4D9CCE4173E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDD681B9-BB22-47F0-AFF0-29E25880FC2F}"/>
   <bookViews>
-    <workbookView xWindow="9855" yWindow="3045" windowWidth="38700" windowHeight="15345" tabRatio="601" xr2:uid="{14AC8030-20A7-4C66-8027-B1BAD1A4B756}"/>
+    <workbookView xWindow="12795" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="601" xr2:uid="{14AC8030-20A7-4C66-8027-B1BAD1A4B756}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="126">
   <si>
     <t>p_0001_19052022_00.bag</t>
   </si>
@@ -374,31 +374,46 @@
     <t>BK</t>
   </si>
   <si>
-    <t>[{"type":"PATIENT","appearances":[{"start":{"frame":164689,"landmarks":{"right_eye":[151,330],"left_eye":[210,310]}},"end":{"frame":165242}}]},{"type":"UNKNOWN","appearances":[{"start":{"frame":165058,"landmarks":{"right_eye":[17,93],"left_eye":[30,89]}},"end":{"frame":165079}},{"start":{"frame":165106,"landmarks":{"right_eye":[35,145],"left_eye":[47,141]}},"end":{"frame":165169}}]},{"type":"STAFF","appearances":[{"start":{"frame":164689,"landmarks":{"right_eye":[126,182],"left_eye":[150,169],"nose":[146,190],"mouth_right":[144,205],"mouth_left":[163,197]}},"end":{"frame":164752}}]}]</t>
-  </si>
-  <si>
-    <t>[{"type":"PATIENT","appearances":[{"start":{"frame":5173,"landmarks":{"mouth_left":[46,38],"nose":[55,0]}},"end":{"frame":5295}}]},{"type":"STAFF","appearances":[{"start":{"frame":5130,"landmarks":{"left_eye":[1214,26],"nose":[1152,18]}},"end":{"frame":5190}}]}]</t>
-  </si>
-  <si>
-    <t>[{"type":"PATIENT","appearances":[{"start":{"frame":175008,"landmarks":{"right_eye":[715,221],"nose":[716,237]}},"end":{"frame":175185}}]},{"type":"STAFF","appearances":[{"start":{"frame":174933,"landmarks":{"right_eye":[180,23],"left_eye":[224,37],"nose":[201,45],"mouth_right":[174,72],"mouth_left":[210,82]}},"end":{"frame":174987}},{"start":{"frame":175053,"landmarks":{"left_eye":[152,466],"nose":[149,482]}},"end":{"frame":175069}}]}]</t>
-  </si>
-  <si>
     <t>[{"start_frame":9989,"end_frame":10024}]</t>
   </si>
   <si>
-    <t>[{"type":"STAFF","appearances":[{"start":{"frame":26038,"landmarks":{"left_eye":[850,24],"nose":[833,28]}},"end":{"frame":26085}}]}]</t>
-  </si>
-  <si>
-    <t>v</t>
-  </si>
-  <si>
-    <t>[{"type":"STAFF","appearances":[{"start":{"frame":394,"landmarks":{"left_eye":[443,55],"right_eye":[435,52],"nose":[437,58]}},"end":{"frame":429}}]}]</t>
-  </si>
-  <si>
     <t>[{"start_frame":5143,"end_frame":5150,"degree":1},{"start_frame":5151,"end_frame":5185,"degree":2},{"start_frame":5151,"end_frame":5206,"degree":2},{"start_frame":5207,"end_frame":5307,"degree":2},{"start_frame":5208,"end_frame":5398,"degree":1}]</t>
   </si>
   <si>
     <t>[{"type":"STAFF","appearances":[{"start":{"frame":115,"landmarks":{"mouth_right":[248,465],"mouth_left":[227,479]}},"end":{"frame":229}},{"start":{"frame":257,"landmarks":{"mouth_right":[252,475]}},"end":{"frame":281}}]},{"type":"PATIENT","appearances":[{"start":{"frame":796,"landmarks":{"left_eye":[666,-3],"nose":[636,2],"mouth_right":[626,14],"mouth_left":[645,25]}},"end":{"frame":841}}]}]</t>
+  </si>
+  <si>
+    <t>[{"type":"STAFF","appearances":[{"start":{"frame":26038,"landmarks":{"left_eye":[850,24],"nose":[833,28]}},"end":{"frame":26078}},{"start":{"frame":26079,"landmarks":{"left_eye":[890,18],"nose":[869,15]}},"end":{"frame":26085}}]}]</t>
+  </si>
+  <si>
+    <t>[{"start_frame":10001,"end_frame":10002,"degree":2},{"start_frame":10003,"end_frame":10021,"degree":3},{"start_frame":10022,"end_frame":10024,"degree":2},{"start_frame":10025,"end_frame":10025,"degree":1}]</t>
+  </si>
+  <si>
+    <t>[{"type":"PATIENT","appearances":[{"start":{"frame":5173,"landmarks":{"mouth_left":[46,38],"nose":[55,0]}},"end":{"frame":5295}}]},{"type":"STAFF","appearances":[{"start":{"frame":5127,"landmarks":{"left_eye":[1209,-2],"nose":[1146,-3]}},"end":{"frame":5190}}]}]</t>
+  </si>
+  <si>
+    <t>[{"type":"PATIENT","appearances":[{"start":{"frame":174998,"landmarks":{"right_eye":[744,217],"nose":[740,230]}},"end":{"frame":175185}}]},{"type":"STAFF","appearances":[{"start":{"frame":174933,"landmarks":{"right_eye":[180,23],"left_eye":[224,37],"nose":[201,45],"mouth_right":[174,72],"mouth_left":[210,82]}},"end":{"frame":174989}},{"start":{"frame":175051,"landmarks":{"left_eye":[164,466],"nose":[162,486]}},"end":{"frame":175070}}]}]</t>
+  </si>
+  <si>
+    <t>[{"type":"PATIENT","appearances":[{"start":{"frame":164689,"landmarks":{"right_eye":[151,330],"left_eye":[210,310]}},"end":{"frame":165242}}]},{"type":"UNKNOWN","appearances":[{"start":{"frame":165056,"landmarks":{"right_eye":[-2,101],"left_eye":[9,97],"nose":[6,108]}},"end":{"frame":165087}},{"start":{"frame":165088,"landmarks":{"right_eye":[24,108],"left_eye":[37,106],"nose":[31,115]}},"end":{"frame":165169}},{"start":{"frame":165106,"landmarks":{"right_eye":[35,145],"left_eye":[47,141]}},"end":{"frame":165169}}]},{"type":"STAFF","appearances":[{"start":{"frame":164689,"landmarks":{"right_eye":[126,182],"left_eye":[150,169],"nose":[146,190],"mouth_right":[144,205],"mouth_left":[163,197]}},"end":{"frame":164755}},{"start":{"frame":165001,"landmarks":{"nose":[256,0],"mouth_right":[266,10],"mouth_left":[275,-1]}},"end":{"frame":165012}}]}]</t>
+  </si>
+  <si>
+    <t>[{"start_frame":404,"end_frame":458}]</t>
+  </si>
+  <si>
+    <t>[{"type":"STAFF","appearances":[{"start":{"frame":394,"landmarks":{"left_eye":[443,55],"right_eye":[435,52],"nose":[437,58]}},"end":{"frame":420}},{"start":{"frame":424,"landmarks":{"left_eye":[424,75],"right_eye":[415,72],"nose":[419,80]}},"end":{"frame":427}},{"start":{"frame":429,"landmarks":{"left_eye":[435,48],"right_eye":[425,46],"nose":[430,53]}},"end":{"frame":431}}]}]</t>
+  </si>
+  <si>
+    <t>[{"start_frame":155,"end_frame":162,"degree":3},{"start_frame":163,"end_frame":177,"degree":2},{"start_frame":178,"end_frame":180,"degree":1},{"start_frame":187,"end_frame":191,"degree":1},{"start_frame":192,"end_frame":219,"degree":2},{"start_frame":220,"end_frame":223,"degree":1},{"start_frame":224,"end_frame":240,"degree":2},{"start_frame":241,"end_frame":245,"degree":3},{"start_frame":246,"end_frame":338,"degree":2},{"start_frame":339,"end_frame":342,"degree":1},{"start_frame":347,"end_frame":380,"degree":1},{"start_frame":381,"end_frame":393,"degree":2},{"start_frame":394,"end_frame":396,"degree":1},{"start_frame":764,"end_frame":775,"degree":1},{"start_frame":776,"end_frame":804,"degree":2},{"start_frame":805,"end_frame":806,"degree":1},{"start_frame":809,"end_frame":811,"degree":1},{"start_frame":812,"end_frame":823,"degree":2},{"start_frame":824,"end_frame":827,"degree":1},{"start_frame":839,"end_frame":850,"degree":1},{"start_frame":851,"end_frame":888,"degree":2},{"start_frame":889,"end_frame":943,"degree":1},{"start_frame":988,"end_frame":988,"degree":1},{"start_frame":989,"end_frame":989,"degree":2},{"start_frame":990,"end_frame":991,"degree":3}]</t>
+  </si>
+  <si>
+    <t>[{"start_frame":48,"end_frame":154},{"start_frame":992,"end_frame":1054}]</t>
+  </si>
+  <si>
+    <t>[{"start_frame":937,"end_frame":991}]</t>
+  </si>
+  <si>
+    <t>[{"type":"PATIENT","appearances":[{"start":{"frame":153,"landmarks":{"left_eye":[580,384],"nose":[576,400],"mouth_left":[583,411]}},"end":{"frame":164}},{"start":{"frame":381,"landmarks":{"left_eye":[851,158],"nose":[832,177],"mouth_left":[836,191]}},"end":{"frame":393}},{"start":{"frame":394,"landmarks":{"left_eye":[838,122],"nose":[813,141],"mouth_left":[816,160]}},"end":{"frame":398}},{"start":{"frame":399,"landmarks":{"left_eye":[836,87],"nose":[810,106],"mouth_left":[809,126]}},"end":{"frame":402}},{"start":{"frame":403,"landmarks":{"left_eye":[843,45],"nose":[814,66],"mouth_left":[814,83]}},"end":{"frame":432}}]}]</t>
   </si>
 </sst>
 </file>
@@ -610,7 +625,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -798,6 +813,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1149,22 +1167,22 @@
   <dimension ref="A1:N75"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B37" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E46" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="M75" sqref="M75"/>
+      <selection pane="bottomRight" activeCell="N80" sqref="N80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="12.875" customWidth="1"/>
-    <col min="5" max="5" width="24.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.375" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="12.85546875" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="11" width="20" customWidth="1"/>
     <col min="12" max="12" width="20" style="10" customWidth="1"/>
     <col min="13" max="13" width="20" customWidth="1"/>
-    <col min="14" max="16384" width="9.125" style="1"/>
+    <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1613,7 +1631,7 @@
       <c r="K15" s="11"/>
       <c r="L15" s="11"/>
       <c r="M15" s="13" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
@@ -1836,19 +1854,21 @@
       <c r="E24" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
+      <c r="F24" s="32">
+        <v>174933</v>
+      </c>
+      <c r="G24" s="32">
+        <v>175185</v>
+      </c>
       <c r="H24" s="33"/>
       <c r="I24" s="34"/>
       <c r="J24" s="35"/>
       <c r="K24" s="35"/>
       <c r="L24" s="35"/>
       <c r="M24" s="57" t="s">
-        <v>114</v>
-      </c>
-      <c r="N24" s="63" t="s">
-        <v>117</v>
-      </c>
+        <v>118</v>
+      </c>
+      <c r="N24" s="63"/>
     </row>
     <row r="25" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A25" s="28">
@@ -2035,21 +2055,23 @@
       <c r="E32" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
+      <c r="F32" s="32">
+        <v>4860</v>
+      </c>
+      <c r="G32" s="32">
+        <v>5398</v>
+      </c>
       <c r="H32" s="62" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="I32" s="34"/>
       <c r="J32" s="35"/>
       <c r="K32" s="35"/>
       <c r="L32" s="35"/>
       <c r="M32" s="57" t="s">
-        <v>113</v>
-      </c>
-      <c r="N32" s="63" t="s">
         <v>117</v>
       </c>
+      <c r="N32" s="63"/>
     </row>
     <row r="33" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A33" s="27">
@@ -2177,19 +2199,23 @@
       <c r="E38" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="62"/>
+      <c r="F38" s="32">
+        <v>9655</v>
+      </c>
+      <c r="G38" s="32">
+        <v>10025</v>
+      </c>
+      <c r="H38" s="62" t="s">
+        <v>116</v>
+      </c>
       <c r="I38" s="34"/>
       <c r="J38" s="57" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="K38" s="35"/>
       <c r="L38" s="35"/>
       <c r="M38" s="35"/>
-      <c r="N38" s="63" t="s">
-        <v>117</v>
-      </c>
+      <c r="N38" s="63"/>
     </row>
     <row r="39" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A39" s="26">
@@ -2245,19 +2271,21 @@
       <c r="E41" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="F41" s="3"/>
-      <c r="G41" s="3"/>
+      <c r="F41" s="3">
+        <v>26038</v>
+      </c>
+      <c r="G41" s="3">
+        <v>26300</v>
+      </c>
       <c r="H41" s="17"/>
       <c r="I41" s="4"/>
       <c r="J41" s="11"/>
       <c r="K41" s="11"/>
       <c r="L41" s="11"/>
       <c r="M41" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="N41" s="63" t="s">
-        <v>117</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="N41" s="63"/>
     </row>
     <row r="42" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
       <c r="A42" s="54">
@@ -2680,7 +2708,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="26">
         <v>32</v>
       </c>
@@ -2701,7 +2729,7 @@
       <c r="L60" s="11"/>
       <c r="M60" s="11"/>
     </row>
-    <row r="61" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="47">
         <v>33</v>
       </c>
@@ -2724,7 +2752,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="62" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="26">
         <v>34</v>
       </c>
@@ -2747,7 +2775,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="63" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="26">
         <v>34</v>
       </c>
@@ -2768,7 +2796,7 @@
       <c r="L63" s="11"/>
       <c r="M63" s="11"/>
     </row>
-    <row r="64" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="47">
         <v>35</v>
       </c>
@@ -2791,7 +2819,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="65" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="26">
         <v>36</v>
       </c>
@@ -2801,21 +2829,25 @@
       <c r="E65" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
+      <c r="F65" s="3">
+        <v>384</v>
+      </c>
+      <c r="G65" s="3">
+        <v>950</v>
+      </c>
       <c r="H65" s="17"/>
       <c r="I65" s="4"/>
-      <c r="J65" s="11"/>
+      <c r="J65" s="13" t="s">
+        <v>120</v>
+      </c>
       <c r="K65" s="11"/>
       <c r="L65" s="11"/>
       <c r="M65" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="N65" s="63" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+      <c r="N65" s="63"/>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="54">
         <v>37</v>
       </c>
@@ -2838,7 +2870,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="67" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="26">
         <v>37</v>
       </c>
@@ -2861,7 +2893,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="68" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="26">
         <v>37</v>
       </c>
@@ -2884,7 +2916,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="69" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="28">
         <v>37</v>
       </c>
@@ -2908,7 +2940,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="26">
         <v>38</v>
       </c>
@@ -2918,8 +2950,12 @@
       <c r="E70" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
+      <c r="F70" s="3">
+        <v>22</v>
+      </c>
+      <c r="G70" s="3">
+        <v>714</v>
+      </c>
       <c r="H70" s="17"/>
       <c r="I70" s="4"/>
       <c r="J70" s="11"/>
@@ -2928,11 +2964,8 @@
       <c r="M70" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="N70" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="26">
         <v>38</v>
       </c>
@@ -2951,7 +2984,7 @@
       <c r="L71" s="11"/>
       <c r="M71" s="11"/>
     </row>
-    <row r="72" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="47">
         <v>39</v>
       </c>
@@ -2970,7 +3003,7 @@
       <c r="L72" s="46"/>
       <c r="M72" s="46"/>
     </row>
-    <row r="73" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="26">
         <v>40</v>
       </c>
@@ -2989,7 +3022,7 @@
       <c r="L73" s="11"/>
       <c r="M73" s="11"/>
     </row>
-    <row r="74" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="54">
         <v>41</v>
       </c>
@@ -2999,20 +3032,28 @@
       <c r="E74" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="F74" s="32"/>
-      <c r="G74" s="32"/>
+      <c r="F74" s="32">
+        <v>48</v>
+      </c>
+      <c r="G74" s="32">
+        <v>1054</v>
+      </c>
       <c r="H74" s="62" t="s">
-        <v>88</v>
-      </c>
-      <c r="I74" s="34"/>
-      <c r="J74" s="35"/>
+        <v>122</v>
+      </c>
+      <c r="I74" s="64" t="s">
+        <v>123</v>
+      </c>
+      <c r="J74" s="57" t="s">
+        <v>124</v>
+      </c>
       <c r="K74" s="35"/>
       <c r="L74" s="35"/>
       <c r="M74" s="57" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="28">
         <v>41</v>
       </c>
@@ -3044,7 +3085,7 @@
         <v>93</v>
       </c>
       <c r="M75" s="14" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add debugging prints for final testing and try different config values
</commit_message>
<xml_diff>
--- a/dataset_metadata.xlsx
+++ b/dataset_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uibes-my.sharepoint.com/personal/agc968_id_uib_eu/Documents/TFG/GEEIA-TFG-DFU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="209" documentId="8_{D3773089-7DAF-44F1-9F4B-4D9CCE4173E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DDD681B9-BB22-47F0-AFF0-29E25880FC2F}"/>
+  <xr:revisionPtr revIDLastSave="238" documentId="8_{D3773089-7DAF-44F1-9F4B-4D9CCE4173E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30D7E28D-D7D9-4C16-8093-6FA97D76F6A0}"/>
   <bookViews>
-    <workbookView xWindow="12795" yWindow="0" windowWidth="26010" windowHeight="20985" tabRatio="601" xr2:uid="{14AC8030-20A7-4C66-8027-B1BAD1A4B756}"/>
+    <workbookView xWindow="5820" yWindow="4050" windowWidth="38700" windowHeight="15345" tabRatio="601" xr2:uid="{14AC8030-20A7-4C66-8027-B1BAD1A4B756}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -380,9 +380,6 @@
     <t>[{"start_frame":5143,"end_frame":5150,"degree":1},{"start_frame":5151,"end_frame":5185,"degree":2},{"start_frame":5151,"end_frame":5206,"degree":2},{"start_frame":5207,"end_frame":5307,"degree":2},{"start_frame":5208,"end_frame":5398,"degree":1}]</t>
   </si>
   <si>
-    <t>[{"type":"STAFF","appearances":[{"start":{"frame":115,"landmarks":{"mouth_right":[248,465],"mouth_left":[227,479]}},"end":{"frame":229}},{"start":{"frame":257,"landmarks":{"mouth_right":[252,475]}},"end":{"frame":281}}]},{"type":"PATIENT","appearances":[{"start":{"frame":796,"landmarks":{"left_eye":[666,-3],"nose":[636,2],"mouth_right":[626,14],"mouth_left":[645,25]}},"end":{"frame":841}}]}]</t>
-  </si>
-  <si>
     <t>[{"type":"STAFF","appearances":[{"start":{"frame":26038,"landmarks":{"left_eye":[850,24],"nose":[833,28]}},"end":{"frame":26078}},{"start":{"frame":26079,"landmarks":{"left_eye":[890,18],"nose":[869,15]}},"end":{"frame":26085}}]}]</t>
   </si>
   <si>
@@ -413,7 +410,10 @@
     <t>[{"start_frame":937,"end_frame":991}]</t>
   </si>
   <si>
-    <t>[{"type":"PATIENT","appearances":[{"start":{"frame":153,"landmarks":{"left_eye":[580,384],"nose":[576,400],"mouth_left":[583,411]}},"end":{"frame":164}},{"start":{"frame":381,"landmarks":{"left_eye":[851,158],"nose":[832,177],"mouth_left":[836,191]}},"end":{"frame":393}},{"start":{"frame":394,"landmarks":{"left_eye":[838,122],"nose":[813,141],"mouth_left":[816,160]}},"end":{"frame":398}},{"start":{"frame":399,"landmarks":{"left_eye":[836,87],"nose":[810,106],"mouth_left":[809,126]}},"end":{"frame":402}},{"start":{"frame":403,"landmarks":{"left_eye":[843,45],"nose":[814,66],"mouth_left":[814,83]}},"end":{"frame":432}}]}]</t>
+    <t>[{"type":"PATIENT","appearances":[{"start":{"frame":153,"landmarks":{"left_eye":[580,384],"nose":[576,400],"mouth_left":[583,411]},"orientation":"TB"},"end":{"frame":164}},{"start":{"frame":381,"landmarks":{"left_eye":[851,158],"nose":[832,177],"mouth_left":[836,191]},"orientation":"TB"},"end":{"frame":393}},{"start":{"frame":394,"landmarks":{"left_eye":[838,122],"nose":[813,141],"mouth_left":[816,160]},"orientation":"TB"},"end":{"frame":398}},{"start":{"frame":399,"landmarks":{"left_eye":[836,87],"nose":[810,106],"mouth_left":[809,126]},"orientation":"TB"},"end":{"frame":402}},{"start":{"frame":403,"landmarks":{"left_eye":[843,45],"nose":[814,66],"mouth_left":[814,83]},"orientation":"TB"},"end":{"frame":434}}]}]</t>
+  </si>
+  <si>
+    <t>[{"type":"STAFF","appearances":[{"start":{"frame":115,"landmarks":{"mouth_right":[248,465],"mouth_left":[227,479]},"orientation":"BT"},"end":{"frame":229}},{"start":{"frame":257,"landmarks":{"mouth_right":[252,475]},"orientation":"BT"},"end":{"frame":281}}]},{"type":"PATIENT","appearances":[{"start":{"frame":794,"landmarks":{"mouth_right":[624,-3],"mouth_left":[643,6]},"orientation":"TB"},"end":{"frame":841}},{"start":{"frame":933,"landmarks":{"left_eye":[590,99]},"orientation":"TB"},"end":{"frame":940}}]}]</t>
   </si>
 </sst>
 </file>
@@ -451,14 +451,14 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -625,175 +625,163 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="fill" vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="fill" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="fill" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -808,14 +796,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="fill" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="fill"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1166,1926 +1160,1925 @@
   </sheetPr>
   <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E46" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B52" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="N80" sqref="N80"/>
+      <selection pane="bottomRight" activeCell="M75" sqref="M75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="12.85546875" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="20" customWidth="1"/>
-    <col min="12" max="12" width="20" style="10" customWidth="1"/>
-    <col min="13" max="13" width="20" customWidth="1"/>
+    <col min="1" max="4" width="12.140625" customWidth="1"/>
+    <col min="5" max="5" width="23.5703125" style="62" customWidth="1"/>
+    <col min="6" max="7" width="15" style="2" customWidth="1"/>
+    <col min="8" max="11" width="17.85546875" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="17.85546875" customWidth="1"/>
     <col min="14" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="21" t="s">
+      <c r="E1" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="I1" s="21" t="s">
+      <c r="I1" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="J1" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="L1" s="23" t="s">
+      <c r="L1" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="8" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="25">
+    <row r="2" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="10">
         <v>53</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="11">
         <v>65879</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="11">
         <v>66205</v>
       </c>
-      <c r="H2" s="17"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-    </row>
-    <row r="3" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A3" s="29">
+      <c r="H2" s="12"/>
+      <c r="I2" s="13"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+    </row>
+    <row r="3" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
         <v>2</v>
       </c>
-      <c r="B3" s="30">
+      <c r="B3" s="16">
         <v>55</v>
       </c>
-      <c r="C3" s="30" t="s">
+      <c r="C3" s="16" t="s">
         <v>107</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="32">
+      <c r="F3" s="17">
         <v>16120</v>
       </c>
-      <c r="G3" s="32">
+      <c r="G3" s="17">
         <v>16553</v>
       </c>
-      <c r="H3" s="33"/>
-      <c r="I3" s="34"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="35"/>
-      <c r="L3" s="35"/>
-      <c r="M3" s="35"/>
-    </row>
-    <row r="4" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="25">
+      <c r="H3" s="18"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
+    </row>
+    <row r="4" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="15" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="61" t="s">
         <v>2</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="11">
         <v>1412</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="11">
         <v>1924</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="I4" s="4"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-      <c r="L4" s="11"/>
-      <c r="M4" s="11"/>
-    </row>
-    <row r="5" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A5" s="36">
+      <c r="I4" s="13"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+    </row>
+    <row r="5" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="22">
         <v>2</v>
       </c>
-      <c r="B5" s="37"/>
-      <c r="C5" s="37"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="16" t="s">
+      <c r="B5" s="23"/>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="60" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="24">
         <v>36790</v>
       </c>
-      <c r="G5" s="7">
+      <c r="G5" s="24">
         <v>37041</v>
       </c>
-      <c r="H5" s="19" t="s">
+      <c r="H5" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="I5" s="38"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
-      <c r="M5" s="39"/>
-    </row>
-    <row r="6" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="40">
+      <c r="I5" s="26"/>
+      <c r="J5" s="27"/>
+      <c r="K5" s="27"/>
+      <c r="L5" s="27"/>
+      <c r="M5" s="27"/>
+    </row>
+    <row r="6" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="28">
         <v>3</v>
       </c>
-      <c r="B6" s="41">
+      <c r="B6" s="29">
         <v>40</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="29" t="s">
         <v>108</v>
       </c>
       <c r="E6" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="43">
+      <c r="F6" s="30">
         <v>1375</v>
       </c>
-      <c r="G6" s="43">
+      <c r="G6" s="30">
         <v>1592</v>
       </c>
-      <c r="H6" s="44"/>
-      <c r="I6" s="45"/>
-      <c r="J6" s="46"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="46"/>
-    </row>
-    <row r="7" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="26">
+      <c r="H6" s="31"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="33"/>
+      <c r="L6" s="33"/>
+      <c r="M6" s="33"/>
+    </row>
+    <row r="7" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="34">
         <v>4</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="35">
         <v>63</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="61" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="11">
         <v>126626</v>
       </c>
-      <c r="G7" s="3">
+      <c r="G7" s="11">
         <v>127070</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="I7" s="4"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-      <c r="L7" s="13" t="s">
+      <c r="I7" s="13"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="36" t="s">
         <v>87</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="M7" s="37" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="47">
+    <row r="8" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="38">
         <v>5</v>
       </c>
-      <c r="B8" s="48">
+      <c r="B8" s="39">
         <v>56</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="C8" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="D8" s="39" t="s">
         <v>108</v>
       </c>
       <c r="E8" s="42" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="43">
+      <c r="F8" s="30">
         <v>54642</v>
       </c>
-      <c r="G8" s="43">
+      <c r="G8" s="30">
         <v>54935</v>
       </c>
-      <c r="H8" s="44"/>
-      <c r="I8" s="45"/>
-      <c r="J8" s="46"/>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="49" t="s">
+      <c r="H8" s="31"/>
+      <c r="I8" s="32"/>
+      <c r="J8" s="33"/>
+      <c r="K8" s="33"/>
+      <c r="L8" s="33"/>
+      <c r="M8" s="40" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="26">
+    <row r="9" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="34">
         <v>6</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="35">
         <v>64</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="61" t="s">
         <v>7</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="11">
         <v>5874</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="11">
         <v>6118</v>
       </c>
-      <c r="H9" s="17"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-      <c r="L9" s="11"/>
-      <c r="M9" s="11"/>
-    </row>
-    <row r="10" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="47">
+      <c r="H9" s="12"/>
+      <c r="I9" s="13"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+    </row>
+    <row r="10" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="38">
         <v>7</v>
       </c>
-      <c r="B10" s="48">
+      <c r="B10" s="39">
         <v>55</v>
       </c>
-      <c r="C10" s="48" t="s">
+      <c r="C10" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="D10" s="48" t="s">
+      <c r="D10" s="39" t="s">
         <v>109</v>
       </c>
       <c r="E10" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="F10" s="43">
+      <c r="F10" s="30">
         <v>47881</v>
       </c>
-      <c r="G10" s="43">
+      <c r="G10" s="30">
         <v>48817</v>
       </c>
-      <c r="H10" s="50" t="s">
+      <c r="H10" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="I10" s="51" t="s">
+      <c r="I10" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="J10" s="46"/>
-      <c r="K10" s="46"/>
-      <c r="L10" s="46"/>
-      <c r="M10" s="46"/>
-    </row>
-    <row r="11" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="26">
+      <c r="J10" s="33"/>
+      <c r="K10" s="33"/>
+      <c r="L10" s="33"/>
+      <c r="M10" s="33"/>
+    </row>
+    <row r="11" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="34">
         <v>8</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="35">
         <v>65</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="61" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11" s="11">
         <v>26297</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="11">
         <v>26477</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="I11" s="4"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11"/>
-      <c r="M11" s="11"/>
-    </row>
-    <row r="12" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="26">
+      <c r="I11" s="13"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+    </row>
+    <row r="12" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="34">
         <v>8</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="15" t="s">
+      <c r="B12" s="35"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="11">
         <v>4188</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="11">
         <v>4523</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="I12" s="4"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-      <c r="L12" s="11"/>
-      <c r="M12" s="11"/>
-    </row>
-    <row r="13" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="26">
+      <c r="I12" s="13"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
+    </row>
+    <row r="13" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="34">
         <v>8</v>
       </c>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="15" t="s">
+      <c r="B13" s="35"/>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="11">
         <v>5622</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="11">
         <v>5895</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="21" t="s">
         <v>82</v>
       </c>
-      <c r="I13" s="4"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
-    </row>
-    <row r="14" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="52">
+      <c r="I13" s="13"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+    </row>
+    <row r="14" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="43">
         <v>9</v>
       </c>
-      <c r="B14" s="53">
+      <c r="B14" s="44">
         <v>65</v>
       </c>
-      <c r="C14" s="53" t="s">
+      <c r="C14" s="44" t="s">
         <v>107</v>
       </c>
-      <c r="D14" s="53" t="s">
+      <c r="D14" s="44" t="s">
         <v>108</v>
       </c>
       <c r="E14" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="F14" s="43">
+      <c r="F14" s="30">
         <v>130416</v>
       </c>
-      <c r="G14" s="43">
+      <c r="G14" s="30">
         <v>130847</v>
       </c>
-      <c r="H14" s="44"/>
-      <c r="I14" s="45"/>
-      <c r="J14" s="46"/>
-      <c r="K14" s="46"/>
-      <c r="L14" s="46"/>
-      <c r="M14" s="46"/>
-    </row>
-    <row r="15" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A15" s="26">
+      <c r="H14" s="31"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="33"/>
+      <c r="K14" s="33"/>
+      <c r="L14" s="33"/>
+      <c r="M14" s="33"/>
+    </row>
+    <row r="15" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="34">
         <v>10</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="35">
         <v>37</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="61" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="11">
         <v>164689</v>
       </c>
-      <c r="G15" s="3">
+      <c r="G15" s="11">
         <v>165242</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="I15" s="4"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="13" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A16" s="47">
+      <c r="I15" s="13"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="36" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="38">
         <v>11</v>
       </c>
-      <c r="B16" s="48">
+      <c r="B16" s="39">
         <v>61</v>
       </c>
-      <c r="C16" s="48" t="s">
+      <c r="C16" s="39" t="s">
         <v>107</v>
       </c>
-      <c r="D16" s="48" t="s">
+      <c r="D16" s="39" t="s">
         <v>108</v>
       </c>
       <c r="E16" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="F16" s="43">
+      <c r="F16" s="30">
         <v>3234</v>
       </c>
-      <c r="G16" s="43">
+      <c r="G16" s="30">
         <v>3570</v>
       </c>
-      <c r="H16" s="44"/>
-      <c r="I16" s="45" t="s">
+      <c r="H16" s="31"/>
+      <c r="I16" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="J16" s="46"/>
-      <c r="K16" s="46"/>
-      <c r="L16" s="46"/>
-      <c r="M16" s="46"/>
-    </row>
-    <row r="17" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="26">
+      <c r="J16" s="33"/>
+      <c r="K16" s="33"/>
+      <c r="L16" s="33"/>
+      <c r="M16" s="33"/>
+    </row>
+    <row r="17" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="34">
         <v>12</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="35">
         <v>66</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17" s="11">
         <v>124472</v>
       </c>
-      <c r="G17" s="3">
+      <c r="G17" s="11">
         <v>125066</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="I17" s="4"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="13" t="s">
+      <c r="I17" s="13"/>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14"/>
+      <c r="L17" s="14"/>
+      <c r="M17" s="36" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="54">
+    <row r="18" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="45">
         <v>13</v>
       </c>
-      <c r="B18" s="55">
+      <c r="B18" s="46">
         <v>55</v>
       </c>
-      <c r="C18" s="55" t="s">
+      <c r="C18" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="D18" s="55" t="s">
+      <c r="D18" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="E18" s="31" t="s">
+      <c r="E18" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="F18" s="32">
+      <c r="F18" s="17">
         <v>88733</v>
       </c>
-      <c r="G18" s="32">
+      <c r="G18" s="17">
         <v>89258</v>
       </c>
-      <c r="H18" s="33"/>
-      <c r="I18" s="34"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="35"/>
-      <c r="L18" s="35"/>
-      <c r="M18" s="35"/>
-    </row>
-    <row r="19" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="26">
+      <c r="H18" s="18"/>
+      <c r="I18" s="19"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
+      <c r="L18" s="20"/>
+      <c r="M18" s="20"/>
+    </row>
+    <row r="19" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="34">
         <v>13</v>
       </c>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="15" t="s">
+      <c r="B19" s="35"/>
+      <c r="C19" s="35"/>
+      <c r="D19" s="35"/>
+      <c r="E19" s="61" t="s">
         <v>17</v>
       </c>
-      <c r="F19" s="3">
+      <c r="F19" s="11">
         <v>14072</v>
       </c>
-      <c r="G19" s="3">
+      <c r="G19" s="11">
         <v>14647</v>
       </c>
-      <c r="H19" s="18" t="s">
+      <c r="H19" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-    </row>
-    <row r="20" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="28">
+      <c r="I19" s="13"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+    </row>
+    <row r="20" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="47">
         <v>13</v>
       </c>
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="16" t="s">
+      <c r="B20" s="48"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="56"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="39"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="39"/>
-      <c r="M20" s="39"/>
-    </row>
-    <row r="21" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A21" s="27">
+      <c r="F20" s="24"/>
+      <c r="G20" s="24"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="27"/>
+      <c r="L20" s="27"/>
+      <c r="M20" s="27"/>
+    </row>
+    <row r="21" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="50">
         <v>14</v>
       </c>
-      <c r="B21" s="6">
+      <c r="B21" s="51">
         <v>54</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="51" t="s">
         <v>107</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-    </row>
-    <row r="22" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="27">
+      <c r="F21" s="11"/>
+      <c r="G21" s="11"/>
+      <c r="H21" s="12"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+    </row>
+    <row r="22" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="50">
         <v>14</v>
       </c>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="15" t="s">
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="61" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="18" t="s">
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="I22" s="4"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-    </row>
-    <row r="23" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="27">
+      <c r="I22" s="13"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="14"/>
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+    </row>
+    <row r="23" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="50">
         <v>14</v>
       </c>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="6"/>
-      <c r="E23" s="15" t="s">
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="18" t="s">
+      <c r="F23" s="11"/>
+      <c r="G23" s="11"/>
+      <c r="H23" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="I23" s="4"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="13" t="s">
+      <c r="I23" s="13"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="36" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A24" s="54">
+    <row r="24" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="45">
         <v>15</v>
       </c>
-      <c r="B24" s="55">
+      <c r="B24" s="46">
         <v>71</v>
       </c>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55" t="s">
+      <c r="C24" s="46"/>
+      <c r="D24" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="E24" s="31" t="s">
+      <c r="E24" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="32">
+      <c r="F24" s="17">
         <v>174933</v>
       </c>
-      <c r="G24" s="32">
+      <c r="G24" s="17">
         <v>175185</v>
       </c>
-      <c r="H24" s="33"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="35"/>
-      <c r="L24" s="35"/>
-      <c r="M24" s="57" t="s">
-        <v>118</v>
-      </c>
-      <c r="N24" s="63"/>
-    </row>
-    <row r="25" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="28">
+      <c r="H24" s="18"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="20"/>
+      <c r="K24" s="20"/>
+      <c r="L24" s="20"/>
+      <c r="M24" s="52" t="s">
+        <v>117</v>
+      </c>
+      <c r="N24" s="4"/>
+    </row>
+    <row r="25" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="47">
         <v>15</v>
       </c>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="16" t="s">
+      <c r="B25" s="48"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="19" t="s">
+      <c r="F25" s="24"/>
+      <c r="G25" s="24"/>
+      <c r="H25" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="I25" s="38"/>
-      <c r="J25" s="39"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="39"/>
-      <c r="M25" s="14" t="s">
+      <c r="I25" s="26"/>
+      <c r="J25" s="27"/>
+      <c r="K25" s="27"/>
+      <c r="L25" s="27"/>
+      <c r="M25" s="53" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="27">
+    <row r="26" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="50">
         <v>16</v>
       </c>
-      <c r="B26" s="6">
+      <c r="B26" s="51">
         <v>70</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="E26" s="61" t="s">
         <v>24</v>
       </c>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="17"/>
-      <c r="I26" s="4"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
-    </row>
-    <row r="27" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="27">
+      <c r="F26" s="11"/>
+      <c r="G26" s="11"/>
+      <c r="H26" s="12"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+    </row>
+    <row r="27" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="50">
         <v>16</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="15" t="s">
+      <c r="B27" s="51"/>
+      <c r="C27" s="51"/>
+      <c r="D27" s="51"/>
+      <c r="E27" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="18" t="s">
+      <c r="F27" s="11"/>
+      <c r="G27" s="11"/>
+      <c r="H27" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="I27" s="4"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-    </row>
-    <row r="28" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="58">
+      <c r="I27" s="13"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+    </row>
+    <row r="28" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="54">
         <v>17</v>
       </c>
-      <c r="B28" s="59">
+      <c r="B28" s="55">
         <v>63</v>
       </c>
-      <c r="C28" s="59" t="s">
+      <c r="C28" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="D28" s="59" t="s">
+      <c r="D28" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="E28" s="31" t="s">
+      <c r="E28" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="33"/>
-      <c r="I28" s="34"/>
-      <c r="J28" s="35"/>
-      <c r="K28" s="35"/>
-      <c r="L28" s="35"/>
-      <c r="M28" s="57" t="s">
+      <c r="F28" s="17"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="20"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="20"/>
+      <c r="M28" s="52" t="s">
         <v>86</v>
       </c>
       <c r="N28" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="27">
+    <row r="29" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="50">
         <v>17</v>
       </c>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
-      <c r="E29" s="15" t="s">
+      <c r="B29" s="51"/>
+      <c r="C29" s="51"/>
+      <c r="D29" s="51"/>
+      <c r="E29" s="61" t="s">
         <v>27</v>
       </c>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="13" t="s">
+      <c r="F29" s="11"/>
+      <c r="G29" s="11"/>
+      <c r="H29" s="12"/>
+      <c r="I29" s="13"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="36" t="s">
         <v>86</v>
       </c>
       <c r="N29" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="60">
+    <row r="30" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="56">
         <v>17</v>
       </c>
-      <c r="B30" s="61"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="61"/>
-      <c r="E30" s="16" t="s">
+      <c r="B30" s="57"/>
+      <c r="C30" s="57"/>
+      <c r="D30" s="57"/>
+      <c r="E30" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="19" t="s">
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="I30" s="38"/>
-      <c r="J30" s="39"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="39"/>
-      <c r="M30" s="39"/>
-    </row>
-    <row r="31" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="27">
+      <c r="I30" s="26"/>
+      <c r="J30" s="27"/>
+      <c r="K30" s="27"/>
+      <c r="L30" s="27"/>
+      <c r="M30" s="27"/>
+    </row>
+    <row r="31" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="50">
         <v>18</v>
       </c>
-      <c r="B31" s="6">
+      <c r="B31" s="51">
         <v>69</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D31" s="51" t="s">
         <v>108</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="61" t="s">
         <v>29</v>
       </c>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-    </row>
-    <row r="32" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="58">
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="12"/>
+      <c r="I31" s="13"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+    </row>
+    <row r="32" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A32" s="54">
         <v>19</v>
       </c>
-      <c r="B32" s="59">
+      <c r="B32" s="55">
         <v>87</v>
       </c>
-      <c r="C32" s="59" t="s">
+      <c r="C32" s="55" t="s">
         <v>110</v>
       </c>
-      <c r="D32" s="59" t="s">
+      <c r="D32" s="55" t="s">
         <v>108</v>
       </c>
-      <c r="E32" s="31" t="s">
+      <c r="E32" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="F32" s="32">
+      <c r="F32" s="17">
         <v>4860</v>
       </c>
-      <c r="G32" s="32">
+      <c r="G32" s="17">
         <v>5398</v>
       </c>
-      <c r="H32" s="62" t="s">
+      <c r="H32" s="58" t="s">
         <v>113</v>
       </c>
-      <c r="I32" s="34"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="35"/>
-      <c r="L32" s="35"/>
-      <c r="M32" s="57" t="s">
-        <v>117</v>
-      </c>
-      <c r="N32" s="63"/>
-    </row>
-    <row r="33" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="27">
+      <c r="I32" s="19"/>
+      <c r="J32" s="20"/>
+      <c r="K32" s="20"/>
+      <c r="L32" s="20"/>
+      <c r="M32" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="N32" s="4"/>
+    </row>
+    <row r="33" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="50">
         <v>19</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="15" t="s">
+      <c r="B33" s="51"/>
+      <c r="C33" s="51"/>
+      <c r="D33" s="51"/>
+      <c r="E33" s="61" t="s">
         <v>31</v>
       </c>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="13" t="s">
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="12"/>
+      <c r="I33" s="13"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="36" t="s">
         <v>86</v>
       </c>
       <c r="N33" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A34" s="60">
+    <row r="34" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A34" s="56">
         <v>19</v>
       </c>
-      <c r="B34" s="61"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="16" t="s">
+      <c r="B34" s="57"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="57"/>
+      <c r="E34" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="F34" s="7"/>
-      <c r="G34" s="7"/>
-      <c r="H34" s="19" t="s">
+      <c r="F34" s="24"/>
+      <c r="G34" s="24"/>
+      <c r="H34" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="I34" s="38"/>
-      <c r="J34" s="39"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="39"/>
-      <c r="M34" s="14" t="s">
+      <c r="I34" s="26"/>
+      <c r="J34" s="27"/>
+      <c r="K34" s="27"/>
+      <c r="L34" s="27"/>
+      <c r="M34" s="53" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A35" s="26">
+    <row r="35" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A35" s="34">
         <v>20</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="35">
         <v>59</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="C35" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="61" t="s">
         <v>33</v>
       </c>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
-    </row>
-    <row r="36" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="26">
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="12"/>
+      <c r="I35" s="13"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+    </row>
+    <row r="36" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A36" s="34">
         <v>20</v>
       </c>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="15" t="s">
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="35"/>
+      <c r="E36" s="61" t="s">
         <v>34</v>
       </c>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-    </row>
-    <row r="37" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A37" s="26">
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="12"/>
+      <c r="I36" s="13"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+    </row>
+    <row r="37" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A37" s="34">
         <v>20</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
-      <c r="E37" s="15" t="s">
+      <c r="B37" s="35"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="35"/>
+      <c r="E37" s="61" t="s">
         <v>35</v>
       </c>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="17"/>
-      <c r="I37" s="4"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-      <c r="L37" s="11"/>
-      <c r="M37" s="11"/>
-    </row>
-    <row r="38" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="54">
+      <c r="F37" s="11"/>
+      <c r="G37" s="11"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="13"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
+    </row>
+    <row r="38" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A38" s="45">
         <v>21</v>
       </c>
-      <c r="B38" s="55">
+      <c r="B38" s="46">
         <v>74</v>
       </c>
-      <c r="C38" s="55" t="s">
+      <c r="C38" s="46" t="s">
         <v>110</v>
       </c>
-      <c r="D38" s="55" t="s">
+      <c r="D38" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="E38" s="31" t="s">
+      <c r="E38" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="F38" s="32">
+      <c r="F38" s="17">
         <v>9655</v>
       </c>
-      <c r="G38" s="32">
+      <c r="G38" s="17">
         <v>10025</v>
       </c>
-      <c r="H38" s="62" t="s">
-        <v>116</v>
-      </c>
-      <c r="I38" s="34"/>
-      <c r="J38" s="57" t="s">
+      <c r="H38" s="58" t="s">
+        <v>115</v>
+      </c>
+      <c r="I38" s="19"/>
+      <c r="J38" s="52" t="s">
         <v>112</v>
       </c>
-      <c r="K38" s="35"/>
-      <c r="L38" s="35"/>
-      <c r="M38" s="35"/>
-      <c r="N38" s="63"/>
-    </row>
-    <row r="39" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A39" s="26">
+      <c r="K38" s="20"/>
+      <c r="L38" s="20"/>
+      <c r="M38" s="20"/>
+      <c r="N38" s="4"/>
+    </row>
+    <row r="39" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A39" s="34">
         <v>21</v>
       </c>
-      <c r="B39" s="5"/>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="15" t="s">
+      <c r="B39" s="35"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="35"/>
+      <c r="E39" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-      <c r="L39" s="11"/>
-      <c r="M39" s="11"/>
-    </row>
-    <row r="40" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A40" s="28">
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="14"/>
+      <c r="K39" s="14"/>
+      <c r="L39" s="14"/>
+      <c r="M39" s="14"/>
+    </row>
+    <row r="40" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A40" s="47">
         <v>21</v>
       </c>
-      <c r="B40" s="24"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="16" t="s">
+      <c r="B40" s="48"/>
+      <c r="C40" s="48"/>
+      <c r="D40" s="48"/>
+      <c r="E40" s="60" t="s">
         <v>38</v>
       </c>
-      <c r="F40" s="7"/>
-      <c r="G40" s="7"/>
-      <c r="H40" s="56"/>
-      <c r="I40" s="38"/>
-      <c r="J40" s="39"/>
-      <c r="K40" s="39"/>
-      <c r="L40" s="39"/>
-      <c r="M40" s="39"/>
-    </row>
-    <row r="41" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A41" s="26">
+      <c r="F40" s="24"/>
+      <c r="G40" s="24"/>
+      <c r="H40" s="49"/>
+      <c r="I40" s="26"/>
+      <c r="J40" s="27"/>
+      <c r="K40" s="27"/>
+      <c r="L40" s="27"/>
+      <c r="M40" s="27"/>
+    </row>
+    <row r="41" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A41" s="34">
         <v>22</v>
       </c>
-      <c r="B41" s="5">
+      <c r="B41" s="35">
         <v>78</v>
       </c>
-      <c r="C41" s="5" t="s">
+      <c r="C41" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="E41" s="15" t="s">
+      <c r="E41" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F41" s="11">
         <v>26038</v>
       </c>
-      <c r="G41" s="3">
+      <c r="G41" s="11">
         <v>26300</v>
       </c>
-      <c r="H41" s="17"/>
-      <c r="I41" s="4"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="11"/>
-      <c r="L41" s="11"/>
-      <c r="M41" s="13" t="s">
-        <v>115</v>
-      </c>
-      <c r="N41" s="63"/>
-    </row>
-    <row r="42" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="54">
+      <c r="H41" s="12"/>
+      <c r="I41" s="13"/>
+      <c r="J41" s="14"/>
+      <c r="K41" s="14"/>
+      <c r="L41" s="14"/>
+      <c r="M41" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="N41" s="4"/>
+    </row>
+    <row r="42" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A42" s="45">
         <v>23</v>
       </c>
-      <c r="B42" s="55">
+      <c r="B42" s="46">
         <v>82</v>
       </c>
-      <c r="C42" s="55" t="s">
+      <c r="C42" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="D42" s="55" t="s">
+      <c r="D42" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="E42" s="31" t="s">
+      <c r="E42" s="59" t="s">
         <v>40</v>
       </c>
-      <c r="F42" s="32"/>
-      <c r="G42" s="32"/>
-      <c r="H42" s="62" t="s">
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="I42" s="34"/>
-      <c r="J42" s="35"/>
-      <c r="K42" s="35"/>
-      <c r="L42" s="35"/>
-      <c r="M42" s="35"/>
-    </row>
-    <row r="43" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A43" s="26">
+      <c r="I42" s="19"/>
+      <c r="J42" s="20"/>
+      <c r="K42" s="20"/>
+      <c r="L42" s="20"/>
+      <c r="M42" s="20"/>
+    </row>
+    <row r="43" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="34">
         <v>23</v>
       </c>
-      <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
-      <c r="E43" s="15" t="s">
+      <c r="B43" s="35"/>
+      <c r="C43" s="35"/>
+      <c r="D43" s="35"/>
+      <c r="E43" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="18" t="s">
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="I43" s="4"/>
-      <c r="J43" s="11"/>
-      <c r="K43" s="11"/>
-      <c r="L43" s="11"/>
-      <c r="M43" s="11"/>
-    </row>
-    <row r="44" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="28">
+      <c r="I43" s="13"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="14"/>
+      <c r="L43" s="14"/>
+      <c r="M43" s="14"/>
+    </row>
+    <row r="44" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A44" s="47">
         <v>23</v>
       </c>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="16" t="s">
+      <c r="B44" s="48"/>
+      <c r="C44" s="48"/>
+      <c r="D44" s="48"/>
+      <c r="E44" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="19" t="s">
+      <c r="F44" s="24"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="I44" s="38"/>
-      <c r="J44" s="39"/>
-      <c r="K44" s="39"/>
-      <c r="L44" s="39"/>
-      <c r="M44" s="39"/>
-    </row>
-    <row r="45" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A45" s="26">
+      <c r="I44" s="26"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
+      <c r="L44" s="27"/>
+      <c r="M44" s="27"/>
+    </row>
+    <row r="45" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="34">
         <v>24</v>
       </c>
-      <c r="B45" s="5">
+      <c r="B45" s="35">
         <v>62</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C45" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="E45" s="15" t="s">
+      <c r="E45" s="61" t="s">
         <v>43</v>
       </c>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="4"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="11"/>
-      <c r="L45" s="11"/>
-      <c r="M45" s="11"/>
-    </row>
-    <row r="46" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A46" s="54">
+      <c r="F45" s="11"/>
+      <c r="G45" s="11"/>
+      <c r="H45" s="12"/>
+      <c r="I45" s="13"/>
+      <c r="J45" s="14"/>
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
+      <c r="M45" s="14"/>
+    </row>
+    <row r="46" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A46" s="45">
         <v>25</v>
       </c>
-      <c r="B46" s="55">
+      <c r="B46" s="46">
         <v>56</v>
       </c>
-      <c r="C46" s="55" t="s">
+      <c r="C46" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="D46" s="55" t="s">
+      <c r="D46" s="46" t="s">
         <v>109</v>
       </c>
-      <c r="E46" s="31" t="s">
+      <c r="E46" s="59" t="s">
         <v>44</v>
       </c>
-      <c r="F46" s="32"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="33"/>
-      <c r="I46" s="34"/>
-      <c r="J46" s="35"/>
-      <c r="K46" s="35"/>
-      <c r="L46" s="35"/>
-      <c r="M46" s="35"/>
-    </row>
-    <row r="47" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A47" s="26">
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="19"/>
+      <c r="J46" s="20"/>
+      <c r="K46" s="20"/>
+      <c r="L46" s="20"/>
+      <c r="M46" s="20"/>
+    </row>
+    <row r="47" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="34">
         <v>25</v>
       </c>
-      <c r="B47" s="5"/>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
-      <c r="E47" s="15" t="s">
+      <c r="B47" s="35"/>
+      <c r="C47" s="35"/>
+      <c r="D47" s="35"/>
+      <c r="E47" s="61" t="s">
         <v>45</v>
       </c>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="17"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-      <c r="L47" s="11"/>
-      <c r="M47" s="11"/>
-    </row>
-    <row r="48" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A48" s="28">
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="12"/>
+      <c r="I47" s="13"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="14"/>
+    </row>
+    <row r="48" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A48" s="47">
         <v>25</v>
       </c>
-      <c r="B48" s="24"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="16" t="s">
+      <c r="B48" s="48"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="60" t="s">
         <v>46</v>
       </c>
-      <c r="F48" s="7"/>
-      <c r="G48" s="7"/>
-      <c r="H48" s="19" t="s">
+      <c r="F48" s="24"/>
+      <c r="G48" s="24"/>
+      <c r="H48" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="I48" s="38"/>
-      <c r="J48" s="39"/>
-      <c r="K48" s="39"/>
-      <c r="L48" s="39"/>
-      <c r="M48" s="39"/>
-    </row>
-    <row r="49" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="26">
+      <c r="I48" s="26"/>
+      <c r="J48" s="27"/>
+      <c r="K48" s="27"/>
+      <c r="L48" s="27"/>
+      <c r="M48" s="27"/>
+    </row>
+    <row r="49" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A49" s="34">
         <v>26</v>
       </c>
-      <c r="B49" s="5">
+      <c r="B49" s="35">
         <v>70</v>
       </c>
-      <c r="C49" s="5" t="s">
+      <c r="C49" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="E49" s="15" t="s">
+      <c r="E49" s="61" t="s">
         <v>47</v>
       </c>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="17"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="11"/>
-      <c r="L49" s="11"/>
-      <c r="M49" s="11"/>
-    </row>
-    <row r="50" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A50" s="54">
+      <c r="F49" s="11"/>
+      <c r="G49" s="11"/>
+      <c r="H49" s="12"/>
+      <c r="I49" s="13"/>
+      <c r="J49" s="14"/>
+      <c r="K49" s="14"/>
+      <c r="L49" s="14"/>
+      <c r="M49" s="14"/>
+    </row>
+    <row r="50" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A50" s="45">
         <v>27</v>
       </c>
-      <c r="B50" s="55">
+      <c r="B50" s="46">
         <v>56</v>
       </c>
-      <c r="C50" s="55" t="s">
+      <c r="C50" s="46" t="s">
         <v>107</v>
       </c>
-      <c r="D50" s="55" t="s">
+      <c r="D50" s="46" t="s">
         <v>108</v>
       </c>
-      <c r="E50" s="31" t="s">
+      <c r="E50" s="59" t="s">
         <v>48</v>
       </c>
-      <c r="F50" s="32"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="33"/>
-      <c r="I50" s="34"/>
-      <c r="J50" s="35"/>
-      <c r="K50" s="35"/>
-      <c r="L50" s="35"/>
-      <c r="M50" s="35"/>
-    </row>
-    <row r="51" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A51" s="26">
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="18"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="20"/>
+      <c r="L50" s="20"/>
+      <c r="M50" s="20"/>
+    </row>
+    <row r="51" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A51" s="34">
         <v>27</v>
       </c>
-      <c r="B51" s="5"/>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
-      <c r="E51" s="15" t="s">
+      <c r="B51" s="35"/>
+      <c r="C51" s="35"/>
+      <c r="D51" s="35"/>
+      <c r="E51" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="F51" s="3"/>
-      <c r="G51" s="3"/>
-      <c r="H51" s="17"/>
-      <c r="I51" s="4"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
-      <c r="L51" s="11"/>
-      <c r="M51" s="11"/>
-    </row>
-    <row r="52" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A52" s="28">
+      <c r="F51" s="11"/>
+      <c r="G51" s="11"/>
+      <c r="H51" s="12"/>
+      <c r="I51" s="13"/>
+      <c r="J51" s="14"/>
+      <c r="K51" s="14"/>
+      <c r="L51" s="14"/>
+      <c r="M51" s="14"/>
+    </row>
+    <row r="52" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="47">
         <v>27</v>
       </c>
-      <c r="B52" s="24"/>
-      <c r="C52" s="24"/>
-      <c r="D52" s="24"/>
-      <c r="E52" s="16" t="s">
+      <c r="B52" s="48"/>
+      <c r="C52" s="48"/>
+      <c r="D52" s="48"/>
+      <c r="E52" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="F52" s="7"/>
-      <c r="G52" s="7"/>
-      <c r="H52" s="19" t="s">
+      <c r="F52" s="24"/>
+      <c r="G52" s="24"/>
+      <c r="H52" s="25" t="s">
         <v>88</v>
       </c>
-      <c r="I52" s="38"/>
-      <c r="J52" s="39"/>
-      <c r="K52" s="39"/>
-      <c r="L52" s="39"/>
-      <c r="M52" s="39"/>
-    </row>
-    <row r="53" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A53" s="26">
+      <c r="I52" s="26"/>
+      <c r="J52" s="27"/>
+      <c r="K52" s="27"/>
+      <c r="L52" s="27"/>
+      <c r="M52" s="27"/>
+    </row>
+    <row r="53" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A53" s="34">
         <v>28</v>
       </c>
-      <c r="B53" s="5">
+      <c r="B53" s="35">
         <v>70</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C53" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="E53" s="15" t="s">
+      <c r="E53" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="17"/>
-      <c r="I53" s="4"/>
-      <c r="J53" s="11"/>
-      <c r="K53" s="11"/>
-      <c r="L53" s="11"/>
-      <c r="M53" s="13" t="s">
+      <c r="F53" s="11"/>
+      <c r="G53" s="11"/>
+      <c r="H53" s="12"/>
+      <c r="I53" s="13"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="14"/>
+      <c r="L53" s="14"/>
+      <c r="M53" s="36" t="s">
         <v>86</v>
       </c>
       <c r="N53" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A54" s="26">
+    <row r="54" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A54" s="34">
         <v>28</v>
       </c>
-      <c r="B54" s="5"/>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
-      <c r="E54" s="15" t="s">
+      <c r="B54" s="35"/>
+      <c r="C54" s="35"/>
+      <c r="D54" s="35"/>
+      <c r="E54" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="4"/>
-      <c r="J54" s="11"/>
-      <c r="K54" s="11"/>
-      <c r="L54" s="11"/>
-      <c r="M54" s="13" t="s">
+      <c r="F54" s="11"/>
+      <c r="G54" s="11"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="13"/>
+      <c r="J54" s="14"/>
+      <c r="K54" s="14"/>
+      <c r="L54" s="14"/>
+      <c r="M54" s="36" t="s">
         <v>86</v>
       </c>
       <c r="N54" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A55" s="26">
+    <row r="55" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A55" s="34">
         <v>28</v>
       </c>
-      <c r="B55" s="5"/>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5"/>
-      <c r="E55" s="15" t="s">
+      <c r="B55" s="35"/>
+      <c r="C55" s="35"/>
+      <c r="D55" s="35"/>
+      <c r="E55" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="17"/>
-      <c r="I55" s="4"/>
-      <c r="J55" s="11"/>
-      <c r="K55" s="11"/>
-      <c r="L55" s="11"/>
-      <c r="M55" s="13" t="s">
+      <c r="F55" s="11"/>
+      <c r="G55" s="11"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="13"/>
+      <c r="J55" s="14"/>
+      <c r="K55" s="14"/>
+      <c r="L55" s="14"/>
+      <c r="M55" s="36" t="s">
         <v>86</v>
       </c>
       <c r="N55" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A56" s="47">
+    <row r="56" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A56" s="38">
         <v>29</v>
       </c>
-      <c r="B56" s="48">
+      <c r="B56" s="39">
         <v>44</v>
       </c>
-      <c r="C56" s="48" t="s">
+      <c r="C56" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="D56" s="48" t="s">
+      <c r="D56" s="39" t="s">
         <v>108</v>
       </c>
       <c r="E56" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="F56" s="43"/>
-      <c r="G56" s="43"/>
-      <c r="H56" s="50" t="s">
+      <c r="F56" s="30"/>
+      <c r="G56" s="30"/>
+      <c r="H56" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="I56" s="45"/>
-      <c r="J56" s="46"/>
-      <c r="K56" s="46"/>
-      <c r="L56" s="46"/>
-      <c r="M56" s="46"/>
-    </row>
-    <row r="57" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A57" s="26">
+      <c r="I56" s="32"/>
+      <c r="J56" s="33"/>
+      <c r="K56" s="33"/>
+      <c r="L56" s="33"/>
+      <c r="M56" s="33"/>
+    </row>
+    <row r="57" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A57" s="34">
         <v>30</v>
       </c>
-      <c r="B57" s="5"/>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
-      <c r="E57" s="15" t="s">
+      <c r="B57" s="35"/>
+      <c r="C57" s="35"/>
+      <c r="D57" s="35"/>
+      <c r="E57" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="18" t="s">
+      <c r="F57" s="11"/>
+      <c r="G57" s="11"/>
+      <c r="H57" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="I57" s="4"/>
-      <c r="J57" s="11"/>
-      <c r="K57" s="11"/>
-      <c r="L57" s="11"/>
-      <c r="M57" s="13" t="s">
+      <c r="I57" s="13"/>
+      <c r="J57" s="14"/>
+      <c r="K57" s="14"/>
+      <c r="L57" s="14"/>
+      <c r="M57" s="36" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="58" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="47">
+    <row r="58" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A58" s="38">
         <v>31</v>
       </c>
-      <c r="B58" s="48"/>
-      <c r="C58" s="48"/>
-      <c r="D58" s="48"/>
+      <c r="B58" s="39"/>
+      <c r="C58" s="39"/>
+      <c r="D58" s="39"/>
       <c r="E58" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="F58" s="43"/>
-      <c r="G58" s="43"/>
-      <c r="H58" s="50" t="s">
+      <c r="F58" s="30"/>
+      <c r="G58" s="30"/>
+      <c r="H58" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="I58" s="45"/>
-      <c r="J58" s="46"/>
-      <c r="K58" s="46"/>
-      <c r="L58" s="46"/>
-      <c r="M58" s="46"/>
-    </row>
-    <row r="59" spans="1:14" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A59" s="26">
+      <c r="I58" s="32"/>
+      <c r="J58" s="33"/>
+      <c r="K58" s="33"/>
+      <c r="L58" s="33"/>
+      <c r="M58" s="33"/>
+    </row>
+    <row r="59" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A59" s="34">
         <v>32</v>
       </c>
-      <c r="B59" s="5"/>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
-      <c r="E59" s="15" t="s">
+      <c r="B59" s="35"/>
+      <c r="C59" s="35"/>
+      <c r="D59" s="35"/>
+      <c r="E59" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="F59" s="3"/>
-      <c r="G59" s="3"/>
-      <c r="H59" s="18" t="s">
+      <c r="F59" s="11"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="I59" s="4"/>
-      <c r="J59" s="11"/>
-      <c r="K59" s="11"/>
-      <c r="L59" s="11"/>
-      <c r="M59" s="13" t="s">
+      <c r="I59" s="13"/>
+      <c r="J59" s="14"/>
+      <c r="K59" s="14"/>
+      <c r="L59" s="14"/>
+      <c r="M59" s="36" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A60" s="26">
+    <row r="60" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A60" s="34">
         <v>32</v>
       </c>
-      <c r="B60" s="5"/>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
-      <c r="E60" s="15" t="s">
+      <c r="B60" s="35"/>
+      <c r="C60" s="35"/>
+      <c r="D60" s="35"/>
+      <c r="E60" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="18" t="s">
+      <c r="F60" s="11"/>
+      <c r="G60" s="11"/>
+      <c r="H60" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="I60" s="4"/>
-      <c r="J60" s="11"/>
-      <c r="K60" s="11"/>
-      <c r="L60" s="11"/>
-      <c r="M60" s="11"/>
-    </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A61" s="47">
+      <c r="I60" s="13"/>
+      <c r="J60" s="14"/>
+      <c r="K60" s="14"/>
+      <c r="L60" s="14"/>
+      <c r="M60" s="14"/>
+    </row>
+    <row r="61" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A61" s="38">
         <v>33</v>
       </c>
-      <c r="B61" s="48"/>
-      <c r="C61" s="48"/>
-      <c r="D61" s="48"/>
+      <c r="B61" s="39"/>
+      <c r="C61" s="39"/>
+      <c r="D61" s="39"/>
       <c r="E61" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="F61" s="43"/>
-      <c r="G61" s="43"/>
-      <c r="H61" s="50" t="s">
+      <c r="F61" s="30"/>
+      <c r="G61" s="30"/>
+      <c r="H61" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="I61" s="45"/>
-      <c r="J61" s="46"/>
-      <c r="K61" s="46"/>
-      <c r="L61" s="46"/>
-      <c r="M61" s="49" t="s">
+      <c r="I61" s="32"/>
+      <c r="J61" s="33"/>
+      <c r="K61" s="33"/>
+      <c r="L61" s="33"/>
+      <c r="M61" s="40" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A62" s="26">
+    <row r="62" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A62" s="34">
         <v>34</v>
       </c>
-      <c r="B62" s="5"/>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
-      <c r="E62" s="15" t="s">
+      <c r="B62" s="35"/>
+      <c r="C62" s="35"/>
+      <c r="D62" s="35"/>
+      <c r="E62" s="61" t="s">
         <v>60</v>
       </c>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="18" t="s">
+      <c r="F62" s="11"/>
+      <c r="G62" s="11"/>
+      <c r="H62" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="I62" s="4"/>
-      <c r="J62" s="11"/>
-      <c r="K62" s="11"/>
-      <c r="L62" s="11"/>
-      <c r="M62" s="13" t="s">
+      <c r="I62" s="13"/>
+      <c r="J62" s="14"/>
+      <c r="K62" s="14"/>
+      <c r="L62" s="14"/>
+      <c r="M62" s="36" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A63" s="26">
+    <row r="63" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A63" s="34">
         <v>34</v>
       </c>
-      <c r="B63" s="5"/>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5"/>
-      <c r="E63" s="15" t="s">
+      <c r="B63" s="35"/>
+      <c r="C63" s="35"/>
+      <c r="D63" s="35"/>
+      <c r="E63" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="18" t="s">
+      <c r="F63" s="11"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="I63" s="4"/>
-      <c r="J63" s="11"/>
-      <c r="K63" s="11"/>
-      <c r="L63" s="11"/>
-      <c r="M63" s="11"/>
-    </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A64" s="47">
+      <c r="I63" s="13"/>
+      <c r="J63" s="14"/>
+      <c r="K63" s="14"/>
+      <c r="L63" s="14"/>
+      <c r="M63" s="14"/>
+    </row>
+    <row r="64" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A64" s="38">
         <v>35</v>
       </c>
-      <c r="B64" s="48"/>
-      <c r="C64" s="48"/>
-      <c r="D64" s="48"/>
+      <c r="B64" s="39"/>
+      <c r="C64" s="39"/>
+      <c r="D64" s="39"/>
       <c r="E64" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="F64" s="43"/>
-      <c r="G64" s="43"/>
-      <c r="H64" s="50" t="s">
+      <c r="F64" s="30"/>
+      <c r="G64" s="30"/>
+      <c r="H64" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="I64" s="45"/>
-      <c r="J64" s="46"/>
-      <c r="K64" s="46"/>
-      <c r="L64" s="46"/>
-      <c r="M64" s="49" t="s">
+      <c r="I64" s="32"/>
+      <c r="J64" s="33"/>
+      <c r="K64" s="33"/>
+      <c r="L64" s="33"/>
+      <c r="M64" s="40" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A65" s="26">
+    <row r="65" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A65" s="34">
         <v>36</v>
       </c>
-      <c r="B65" s="5"/>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
-      <c r="E65" s="15" t="s">
+      <c r="B65" s="35"/>
+      <c r="C65" s="35"/>
+      <c r="D65" s="35"/>
+      <c r="E65" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="F65" s="3">
+      <c r="F65" s="11">
         <v>384</v>
       </c>
-      <c r="G65" s="3">
+      <c r="G65" s="11">
         <v>950</v>
       </c>
-      <c r="H65" s="17"/>
-      <c r="I65" s="4"/>
-      <c r="J65" s="13" t="s">
+      <c r="H65" s="12"/>
+      <c r="I65" s="13"/>
+      <c r="J65" s="36" t="s">
+        <v>119</v>
+      </c>
+      <c r="K65" s="14"/>
+      <c r="L65" s="14"/>
+      <c r="M65" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="K65" s="11"/>
-      <c r="L65" s="11"/>
-      <c r="M65" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="N65" s="63"/>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A66" s="54">
+      <c r="N65" s="4"/>
+    </row>
+    <row r="66" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A66" s="45">
         <v>37</v>
       </c>
-      <c r="B66" s="55"/>
-      <c r="C66" s="55"/>
-      <c r="D66" s="55"/>
-      <c r="E66" s="31" t="s">
+      <c r="B66" s="46"/>
+      <c r="C66" s="46"/>
+      <c r="D66" s="46"/>
+      <c r="E66" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="F66" s="32"/>
-      <c r="G66" s="32"/>
-      <c r="H66" s="62" t="s">
+      <c r="F66" s="17"/>
+      <c r="G66" s="17"/>
+      <c r="H66" s="58" t="s">
         <v>88</v>
       </c>
-      <c r="I66" s="34"/>
-      <c r="J66" s="35"/>
-      <c r="K66" s="35"/>
-      <c r="L66" s="35"/>
-      <c r="M66" s="57" t="s">
+      <c r="I66" s="19"/>
+      <c r="J66" s="20"/>
+      <c r="K66" s="20"/>
+      <c r="L66" s="20"/>
+      <c r="M66" s="52" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A67" s="26">
+    <row r="67" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A67" s="34">
         <v>37</v>
       </c>
-      <c r="B67" s="5"/>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
-      <c r="E67" s="15" t="s">
+      <c r="B67" s="35"/>
+      <c r="C67" s="35"/>
+      <c r="D67" s="35"/>
+      <c r="E67" s="61" t="s">
         <v>65</v>
       </c>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
-      <c r="H67" s="18" t="s">
+      <c r="F67" s="11"/>
+      <c r="G67" s="11"/>
+      <c r="H67" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="I67" s="4"/>
-      <c r="J67" s="11"/>
-      <c r="K67" s="11"/>
-      <c r="L67" s="11"/>
-      <c r="M67" s="13" t="s">
+      <c r="I67" s="13"/>
+      <c r="J67" s="14"/>
+      <c r="K67" s="14"/>
+      <c r="L67" s="14"/>
+      <c r="M67" s="36" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A68" s="26">
+    <row r="68" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A68" s="34">
         <v>37</v>
       </c>
-      <c r="B68" s="5"/>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
-      <c r="E68" s="15" t="s">
+      <c r="B68" s="35"/>
+      <c r="C68" s="35"/>
+      <c r="D68" s="35"/>
+      <c r="E68" s="61" t="s">
         <v>66</v>
       </c>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-      <c r="H68" s="18" t="s">
+      <c r="F68" s="11"/>
+      <c r="G68" s="11"/>
+      <c r="H68" s="21" t="s">
         <v>88</v>
       </c>
-      <c r="I68" s="4"/>
-      <c r="J68" s="11"/>
-      <c r="K68" s="11"/>
-      <c r="L68" s="11"/>
-      <c r="M68" s="13" t="s">
+      <c r="I68" s="13"/>
+      <c r="J68" s="14"/>
+      <c r="K68" s="14"/>
+      <c r="L68" s="14"/>
+      <c r="M68" s="36" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A69" s="28">
+    <row r="69" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A69" s="47">
         <v>37</v>
       </c>
-      <c r="B69" s="24"/>
-      <c r="C69" s="24"/>
-      <c r="D69" s="24"/>
-      <c r="E69" s="16" t="s">
+      <c r="B69" s="48"/>
+      <c r="C69" s="48"/>
+      <c r="D69" s="48"/>
+      <c r="E69" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="F69" s="7"/>
-      <c r="G69" s="7"/>
-      <c r="H69" s="56"/>
-      <c r="I69" s="38"/>
-      <c r="J69" s="39"/>
-      <c r="K69" s="39"/>
-      <c r="L69" s="39"/>
-      <c r="M69" s="14" t="s">
+      <c r="F69" s="24"/>
+      <c r="G69" s="24"/>
+      <c r="H69" s="49"/>
+      <c r="I69" s="26"/>
+      <c r="J69" s="27"/>
+      <c r="K69" s="27"/>
+      <c r="L69" s="27"/>
+      <c r="M69" s="53" t="s">
         <v>86</v>
       </c>
       <c r="N69" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A70" s="26">
+    <row r="70" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A70" s="34">
         <v>38</v>
       </c>
-      <c r="B70" s="5"/>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
-      <c r="E70" s="15" t="s">
+      <c r="B70" s="35"/>
+      <c r="C70" s="35"/>
+      <c r="D70" s="35"/>
+      <c r="E70" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="F70" s="3">
+      <c r="F70" s="11">
         <v>22</v>
       </c>
-      <c r="G70" s="3">
+      <c r="G70" s="11">
         <v>714</v>
       </c>
-      <c r="H70" s="17"/>
-      <c r="I70" s="4"/>
-      <c r="J70" s="11"/>
-      <c r="K70" s="11"/>
-      <c r="L70" s="11"/>
-      <c r="M70" s="13" t="s">
+      <c r="H70" s="12"/>
+      <c r="I70" s="13"/>
+      <c r="J70" s="14"/>
+      <c r="K70" s="14"/>
+      <c r="L70" s="14"/>
+      <c r="M70" s="36" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A71" s="26">
+    <row r="71" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A71" s="34">
         <v>38</v>
       </c>
-      <c r="B71" s="5"/>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
-      <c r="E71" s="15" t="s">
+      <c r="B71" s="35"/>
+      <c r="C71" s="35"/>
+      <c r="D71" s="35"/>
+      <c r="E71" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
-      <c r="H71" s="17"/>
-      <c r="I71" s="4"/>
-      <c r="J71" s="11"/>
-      <c r="K71" s="11"/>
-      <c r="L71" s="11"/>
-      <c r="M71" s="11"/>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A72" s="47">
+      <c r="F71" s="11"/>
+      <c r="G71" s="11"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="14"/>
+      <c r="K71" s="14"/>
+      <c r="L71" s="14"/>
+      <c r="M71" s="14"/>
+    </row>
+    <row r="72" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="38">
         <v>39</v>
       </c>
-      <c r="B72" s="48"/>
-      <c r="C72" s="48"/>
-      <c r="D72" s="48"/>
+      <c r="B72" s="39"/>
+      <c r="C72" s="39"/>
+      <c r="D72" s="39"/>
       <c r="E72" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="F72" s="43"/>
-      <c r="G72" s="43"/>
-      <c r="H72" s="44"/>
-      <c r="I72" s="45"/>
-      <c r="J72" s="46"/>
-      <c r="K72" s="46"/>
-      <c r="L72" s="46"/>
-      <c r="M72" s="46"/>
-    </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A73" s="26">
+      <c r="F72" s="30"/>
+      <c r="G72" s="30"/>
+      <c r="H72" s="31"/>
+      <c r="I72" s="32"/>
+      <c r="J72" s="33"/>
+      <c r="K72" s="33"/>
+      <c r="L72" s="33"/>
+      <c r="M72" s="33"/>
+    </row>
+    <row r="73" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A73" s="34">
         <v>40</v>
       </c>
-      <c r="B73" s="5"/>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
-      <c r="E73" s="15" t="s">
+      <c r="B73" s="35"/>
+      <c r="C73" s="35"/>
+      <c r="D73" s="35"/>
+      <c r="E73" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="F73" s="3"/>
-      <c r="G73" s="3"/>
-      <c r="H73" s="17"/>
-      <c r="I73" s="4"/>
-      <c r="J73" s="11"/>
-      <c r="K73" s="11"/>
-      <c r="L73" s="11"/>
-      <c r="M73" s="11"/>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A74" s="54">
+      <c r="F73" s="11"/>
+      <c r="G73" s="11"/>
+      <c r="H73" s="12"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="14"/>
+      <c r="K73" s="14"/>
+      <c r="L73" s="14"/>
+      <c r="M73" s="14"/>
+    </row>
+    <row r="74" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A74" s="45">
         <v>41</v>
       </c>
-      <c r="B74" s="55"/>
-      <c r="C74" s="55"/>
-      <c r="D74" s="55"/>
-      <c r="E74" s="31" t="s">
+      <c r="B74" s="46"/>
+      <c r="C74" s="46"/>
+      <c r="D74" s="46"/>
+      <c r="E74" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="F74" s="32">
+      <c r="F74" s="17">
         <v>48</v>
       </c>
-      <c r="G74" s="32">
+      <c r="G74" s="17">
         <v>1054</v>
       </c>
-      <c r="H74" s="62" t="s">
+      <c r="H74" s="58" t="s">
+        <v>121</v>
+      </c>
+      <c r="I74" s="59" t="s">
         <v>122</v>
       </c>
-      <c r="I74" s="64" t="s">
+      <c r="J74" s="52" t="s">
         <v>123</v>
       </c>
-      <c r="J74" s="57" t="s">
+      <c r="K74" s="20"/>
+      <c r="L74" s="20"/>
+      <c r="M74" s="52" t="s">
         <v>124</v>
       </c>
-      <c r="K74" s="35"/>
-      <c r="L74" s="35"/>
-      <c r="M74" s="57" t="s">
+    </row>
+    <row r="75" spans="1:14" ht="13.5" x14ac:dyDescent="0.25">
+      <c r="A75" s="47">
+        <v>41</v>
+      </c>
+      <c r="B75" s="48"/>
+      <c r="C75" s="48"/>
+      <c r="D75" s="48"/>
+      <c r="E75" s="60" t="s">
+        <v>73</v>
+      </c>
+      <c r="F75" s="24">
+        <v>39</v>
+      </c>
+      <c r="G75" s="24">
+        <v>1196</v>
+      </c>
+      <c r="H75" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="I75" s="60" t="s">
+        <v>89</v>
+      </c>
+      <c r="J75" s="53" t="s">
+        <v>91</v>
+      </c>
+      <c r="K75" s="53" t="s">
+        <v>92</v>
+      </c>
+      <c r="L75" s="53" t="s">
+        <v>93</v>
+      </c>
+      <c r="M75" s="53" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A75" s="28">
-        <v>41</v>
-      </c>
-      <c r="B75" s="24"/>
-      <c r="C75" s="24"/>
-      <c r="D75" s="24"/>
-      <c r="E75" s="16" t="s">
-        <v>73</v>
-      </c>
-      <c r="F75" s="7">
-        <v>39</v>
-      </c>
-      <c r="G75" s="7">
-        <v>1196</v>
-      </c>
-      <c r="H75" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="I75" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="J75" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="K75" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="L75" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="M75" s="14" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>